<commit_message>
Bash: added a row to posts table in DatabaseDesign for actual image data. Database.cs makes all tables at initialization. Wrote a test and functions for meme upload (still in red). TODO: figure out how to pass image data to UploadMeme() - byte[] isn't working so far. Maybe try to convert image to binary first.
</commit_message>
<xml_diff>
--- a/DatabaseDesign/PostTable.xlsx
+++ b/DatabaseDesign/PostTable.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joshua Byron\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\SSU\2019Spring\ETEC2104-OOP\MemeRepository\trunk\DatabaseDesign\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC07A8D5-830B-4F84-81FF-7BCE3E11D3C5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="42" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C47DBDAA-2E77-4D61-9512-F8EF5801A97F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="42" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
   <si>
     <t>Table Name</t>
   </si>
@@ -81,6 +81,12 @@
   </si>
   <si>
     <t>Integer</t>
+  </si>
+  <si>
+    <t>PostData</t>
+  </si>
+  <si>
+    <t>blob</t>
   </si>
 </sst>
 </file>
@@ -528,40 +534,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>2</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -578,25 +585,28 @@
         <v>8</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -613,21 +623,24 @@
         <v>16</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="M3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N3" s="6" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>